<commit_message>
Inclusión de recursos aprovechados
Inclusión de recursos aprovechados
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion15/escaleta_CN_10_15_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion15/escaleta_CN_10_15_CO.xlsx
@@ -19,14 +19,14 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$39</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="256">
   <si>
     <t>Asignatura</t>
   </si>
@@ -782,6 +782,21 @@
   </si>
   <si>
     <t>Recurso F13B-01</t>
+  </si>
+  <si>
+    <t>Las reacciones químicas</t>
+  </si>
+  <si>
+    <t>Calcula las concentraciones de las disoluciones</t>
+  </si>
+  <si>
+    <t>FQ_10_12</t>
+  </si>
+  <si>
+    <t>cambiar desripción y título</t>
+  </si>
+  <si>
+    <t>Calcula porcentajes en masa y en volumen</t>
   </si>
 </sst>
 </file>
@@ -828,7 +843,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -913,6 +928,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -969,7 +996,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1047,16 +1074,35 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1098,31 +1144,39 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1438,9 +1492,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M40" sqref="M40"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,94 +1523,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="M1" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="51"/>
-      <c r="O1" s="39" t="s">
+      <c r="N1" s="58"/>
+      <c r="O1" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="54" t="s">
+      <c r="Q1" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="58" t="s">
+      <c r="R1" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="54" t="s">
+      <c r="S1" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="56" t="s">
+      <c r="T1" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="54" t="s">
+      <c r="U1" s="40" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="46"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="53"/>
       <c r="M2" s="24" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="55"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="41"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -2120,297 +2174,301 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="19" t="s">
+      <c r="F14" s="62"/>
+      <c r="G14" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="63">
         <v>9</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="J14" s="62" t="s">
         <v>214</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7" t="s">
+      <c r="M14" s="64"/>
+      <c r="N14" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18" t="s">
+      <c r="O14" s="62"/>
+      <c r="P14" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="25">
+      <c r="Q14" s="62">
         <v>6</v>
       </c>
-      <c r="R14" s="26" t="s">
+      <c r="R14" s="62" t="s">
         <v>162</v>
       </c>
-      <c r="S14" s="25" t="s">
+      <c r="S14" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="T14" s="27" t="s">
+      <c r="T14" s="62" t="s">
         <v>215</v>
       </c>
-      <c r="U14" s="25" t="s">
+      <c r="U14" s="62" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19" t="s">
+      <c r="F15" s="62"/>
+      <c r="G15" s="62" t="s">
         <v>244</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="63">
         <v>10</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="K15" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7" t="s">
+      <c r="M15" s="64"/>
+      <c r="N15" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18" t="s">
+      <c r="O15" s="62"/>
+      <c r="P15" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="25">
+      <c r="Q15" s="62">
         <v>6</v>
       </c>
-      <c r="R15" s="26" t="s">
+      <c r="R15" s="62" t="s">
         <v>162</v>
       </c>
-      <c r="S15" s="25" t="s">
+      <c r="S15" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="T15" s="27" t="s">
+      <c r="T15" s="62" t="s">
         <v>218</v>
       </c>
-      <c r="U15" s="25" t="s">
+      <c r="U15" s="62" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:21" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="65" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66" t="s">
+        <v>213</v>
+      </c>
+      <c r="H16" s="67">
+        <v>9</v>
+      </c>
+      <c r="I16" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="66" t="s">
+        <v>214</v>
+      </c>
+      <c r="K16" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" s="66" t="s">
+        <v>254</v>
+      </c>
+      <c r="P16" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q16" s="69" t="s">
+        <v>193</v>
+      </c>
+      <c r="R16" s="69" t="s">
+        <v>182</v>
+      </c>
+      <c r="S16" s="69" t="s">
+        <v>251</v>
+      </c>
+      <c r="T16" s="69" t="s">
+        <v>255</v>
+      </c>
+      <c r="U16" s="69" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="65" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="66" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33" t="s">
+      <c r="F17" s="66"/>
+      <c r="G17" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="H17" s="67">
+        <v>10</v>
+      </c>
+      <c r="I17" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="66" t="s">
+        <v>216</v>
+      </c>
+      <c r="K17" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17" s="66" t="s">
+        <v>254</v>
+      </c>
+      <c r="P17" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" s="69" t="s">
+        <v>193</v>
+      </c>
+      <c r="R17" s="69" t="s">
+        <v>182</v>
+      </c>
+      <c r="S17" s="69" t="s">
+        <v>251</v>
+      </c>
+      <c r="T17" s="69" t="s">
+        <v>252</v>
+      </c>
+      <c r="U17" s="69" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="H16" s="34">
+      <c r="H18" s="34">
         <v>11</v>
       </c>
-      <c r="I16" s="35" t="s">
+      <c r="I18" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="33" t="s">
+      <c r="J18" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="K16" s="35" t="s">
+      <c r="K18" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="35" t="s">
+      <c r="L18" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35" t="s">
+      <c r="M18" s="35"/>
+      <c r="N18" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33" t="s">
+      <c r="O18" s="33"/>
+      <c r="P18" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" s="33">
+      <c r="Q18" s="33">
         <v>6</v>
       </c>
-      <c r="R16" s="33" t="s">
+      <c r="R18" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="S16" s="33" t="s">
+      <c r="S18" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="T16" s="33" t="s">
+      <c r="T18" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="U16" s="33" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="H17" s="23">
-        <v>12</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q17" s="25">
-        <v>6</v>
-      </c>
-      <c r="R17" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="S17" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="T17" s="27" t="s">
-        <v>212</v>
-      </c>
-      <c r="U17" s="25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="H18" s="23">
-        <v>13</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q18" s="25">
-        <v>6</v>
-      </c>
-      <c r="R18" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="S18" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="T18" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="U18" s="25" t="s">
+      <c r="U18" s="33" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2425,32 +2483,34 @@
         <v>123</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" s="16"/>
+        <v>131</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>134</v>
+      </c>
       <c r="F19" s="18"/>
       <c r="G19" s="19" t="s">
-        <v>170</v>
+        <v>222</v>
       </c>
       <c r="H19" s="23">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J19" s="20" t="s">
-        <v>171</v>
+        <v>223</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>20</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="N19" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="O19" s="18"/>
       <c r="P19" s="18" t="s">
         <v>19</v>
@@ -2459,134 +2519,132 @@
         <v>6</v>
       </c>
       <c r="R19" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="S19" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="T19" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="U19" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="H20" s="23">
+        <v>13</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q20" s="25">
+        <v>6</v>
+      </c>
+      <c r="R20" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="S20" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="T20" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="U20" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="H21" s="23">
+        <v>14</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="N21" s="7"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="25">
+        <v>6</v>
+      </c>
+      <c r="R21" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="S19" s="25" t="s">
+      <c r="S21" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="T19" s="27" t="s">
+      <c r="T21" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="U19" s="25" t="s">
+      <c r="U21" s="25" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33" t="s">
-        <v>224</v>
-      </c>
-      <c r="H20" s="34">
-        <v>15</v>
-      </c>
-      <c r="I20" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="33" t="s">
-        <v>225</v>
-      </c>
-      <c r="K20" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="L20" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q20" s="33">
-        <v>6</v>
-      </c>
-      <c r="R20" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="S20" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="T20" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="U20" s="33" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33" t="s">
-        <v>245</v>
-      </c>
-      <c r="H21" s="34">
-        <v>16</v>
-      </c>
-      <c r="I21" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="K21" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q21" s="33">
-        <v>6</v>
-      </c>
-      <c r="R21" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="S21" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="T21" s="33" t="s">
-        <v>227</v>
-      </c>
-      <c r="U21" s="33" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2603,20 +2661,20 @@
         <v>135</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F22" s="33"/>
       <c r="G22" s="33" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H22" s="34">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I22" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J22" s="33" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="K22" s="35" t="s">
         <v>20</v>
@@ -2642,7 +2700,7 @@
         <v>163</v>
       </c>
       <c r="T22" s="33" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="U22" s="33" t="s">
         <v>165</v>
@@ -2662,20 +2720,20 @@
         <v>135</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F23" s="33"/>
       <c r="G23" s="33" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="H23" s="34">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I23" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J23" s="33" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="K23" s="35" t="s">
         <v>20</v>
@@ -2701,127 +2759,127 @@
         <v>163</v>
       </c>
       <c r="T23" s="33" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="U23" s="33" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="H24" s="34">
+        <v>17</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="K24" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q24" s="33">
+        <v>6</v>
+      </c>
+      <c r="R24" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="S24" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="T24" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="U24" s="33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="H24" s="23">
+      <c r="F25" s="33"/>
+      <c r="G25" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="H25" s="34">
+        <v>18</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="K25" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" s="35"/>
+      <c r="N25" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="O24" s="18"/>
-      <c r="P24" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q24" s="25">
+      <c r="Q25" s="33">
         <v>6</v>
       </c>
-      <c r="R24" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="S24" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="T24" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="U24" s="25" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="F25" s="18"/>
-      <c r="G25" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="H25" s="23">
-        <v>20</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q25" s="25">
-        <v>6</v>
-      </c>
-      <c r="R25" s="26" t="s">
+      <c r="R25" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="S25" s="25" t="s">
+      <c r="S25" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="T25" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="U25" s="25" t="s">
+      <c r="T25" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="U25" s="33" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2836,27 +2894,53 @@
         <v>123</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F26" s="18"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="5"/>
+      <c r="G26" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="H26" s="23">
+        <v>19</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
+      <c r="N26" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="26"/>
-      <c r="S26" s="25"/>
-      <c r="T26" s="27"/>
-      <c r="U26" s="25"/>
+      <c r="P26" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q26" s="25">
+        <v>6</v>
+      </c>
+      <c r="R26" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="S26" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="T26" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="U26" s="25" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
@@ -2869,34 +2953,34 @@
         <v>123</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="19" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="H27" s="23">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>246</v>
+        <v>160</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>20</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M27" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="N27" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="O27" s="18"/>
       <c r="P27" s="18" t="s">
         <v>19</v>
@@ -2908,13 +2992,13 @@
         <v>162</v>
       </c>
       <c r="S27" s="25" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="T27" s="27" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="U27" s="25" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2931,106 +3015,82 @@
         <v>139</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="F28" s="18"/>
-      <c r="G28" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="H28" s="23">
-        <v>22</v>
-      </c>
-      <c r="I28" s="4" t="s">
+      <c r="G28" s="19"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="25"/>
+      <c r="T28" s="27"/>
+      <c r="U28" s="25"/>
+    </row>
+    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="18"/>
+      <c r="G29" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="H29" s="23">
+        <v>21</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="K29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18" t="s">
+      <c r="L29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N29" s="7"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="25">
+      <c r="Q29" s="25">
         <v>6</v>
       </c>
-      <c r="R28" s="26" t="s">
+      <c r="R29" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="S28" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="T28" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="U28" s="25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="C29" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="H29" s="34">
-        <v>23</v>
-      </c>
-      <c r="I29" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="J29" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="K29" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="L29" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q29" s="33">
-        <v>6</v>
-      </c>
-      <c r="R29" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="S29" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="T29" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="U29" s="33" t="s">
-        <v>165</v>
+      <c r="S29" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="T29" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="U29" s="25" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3044,50 +3104,52 @@
         <v>123</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="E30" s="16"/>
+        <v>139</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>127</v>
+      </c>
       <c r="F30" s="18"/>
       <c r="G30" s="19" t="s">
-        <v>191</v>
+        <v>148</v>
       </c>
       <c r="H30" s="23">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>20</v>
       </c>
       <c r="J30" s="20" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>8</v>
       </c>
       <c r="M30" s="7"/>
       <c r="N30" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O30" s="18"/>
       <c r="P30" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="25" t="s">
-        <v>193</v>
+      <c r="Q30" s="25">
+        <v>6</v>
       </c>
       <c r="R30" s="26" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="S30" s="25" t="s">
-        <v>194</v>
+        <v>163</v>
       </c>
       <c r="T30" s="27" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="U30" s="25" t="s">
-        <v>196</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3106,16 +3168,16 @@
       <c r="E31" s="33"/>
       <c r="F31" s="33"/>
       <c r="G31" s="33" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H31" s="34">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I31" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J31" s="33" t="s">
-        <v>247</v>
+        <v>186</v>
       </c>
       <c r="K31" s="35" t="s">
         <v>20</v>
@@ -3129,7 +3191,7 @@
       </c>
       <c r="O31" s="33"/>
       <c r="P31" s="33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q31" s="33">
         <v>6</v>
@@ -3141,67 +3203,67 @@
         <v>163</v>
       </c>
       <c r="T31" s="33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U31" s="33" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="H32" s="34">
-        <v>26</v>
-      </c>
-      <c r="I32" s="35" t="s">
+      <c r="E32" s="16"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="H32" s="23">
+        <v>24</v>
+      </c>
+      <c r="I32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="K32" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="L32" s="35" t="s">
+      <c r="J32" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35" t="s">
+      <c r="M32" s="7"/>
+      <c r="N32" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="O32" s="33"/>
-      <c r="P32" s="33" t="s">
+      <c r="O32" s="18"/>
+      <c r="P32" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="33">
-        <v>6</v>
-      </c>
-      <c r="R32" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="S32" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="T32" s="33" t="s">
-        <v>205</v>
-      </c>
-      <c r="U32" s="33" t="s">
-        <v>165</v>
+      <c r="Q32" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="R32" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="S32" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="T32" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="U32" s="25" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3220,16 +3282,16 @@
       <c r="E33" s="33"/>
       <c r="F33" s="33"/>
       <c r="G33" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H33" s="34">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I33" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J33" s="33" t="s">
-        <v>197</v>
+        <v>247</v>
       </c>
       <c r="K33" s="35" t="s">
         <v>20</v>
@@ -3255,113 +3317,125 @@
         <v>163</v>
       </c>
       <c r="T33" s="33" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="U33" s="33" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="E34" s="16"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="H34" s="23">
-        <v>28</v>
-      </c>
-      <c r="I34" s="4" t="s">
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="H34" s="34">
+        <v>26</v>
+      </c>
+      <c r="I34" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="K34" s="6" t="s">
+      <c r="J34" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="K34" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L34" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="O34" s="33"/>
+      <c r="P34" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="Q34" s="33">
+        <v>6</v>
+      </c>
+      <c r="R34" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="S34" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="T34" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="U34" s="33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="H35" s="34">
+        <v>27</v>
+      </c>
+      <c r="I35" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K35" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7" t="s">
+      <c r="M35" s="35"/>
+      <c r="N35" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18" t="s">
+      <c r="O35" s="33"/>
+      <c r="P35" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="Q34" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="R34" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="S34" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="T34" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="U34" s="25" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E35" s="16"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="23">
-        <v>29</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J35" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="26"/>
-      <c r="S35" s="25"/>
-      <c r="T35" s="27"/>
-      <c r="U35" s="25"/>
+      <c r="Q35" s="33">
+        <v>6</v>
+      </c>
+      <c r="R35" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="S35" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="T35" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="U35" s="33" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
@@ -3374,50 +3448,50 @@
         <v>123</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E36" s="16"/>
       <c r="F36" s="18"/>
       <c r="G36" s="19" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H36" s="23">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>20</v>
       </c>
       <c r="J36" s="20" t="s">
-        <v>201</v>
+        <v>249</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>8</v>
       </c>
       <c r="M36" s="7"/>
       <c r="N36" s="7" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="O36" s="18"/>
       <c r="P36" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q36" s="25">
-        <v>6</v>
+      <c r="Q36" s="25" t="s">
+        <v>181</v>
       </c>
       <c r="R36" s="26" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="S36" s="25" t="s">
-        <v>235</v>
+        <v>183</v>
       </c>
       <c r="T36" s="27" t="s">
-        <v>241</v>
+        <v>180</v>
       </c>
       <c r="U36" s="25" t="s">
-        <v>237</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3436,92 +3510,148 @@
       <c r="E37" s="16"/>
       <c r="F37" s="18"/>
       <c r="G37" s="19" t="s">
-        <v>198</v>
+        <v>10</v>
       </c>
       <c r="H37" s="23">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J37" s="29" t="s">
-        <v>202</v>
+      <c r="J37" s="20" t="s">
+        <v>200</v>
       </c>
       <c r="K37" s="6" t="s">
         <v>20</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M37" s="7"/>
-      <c r="N37" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="N37" s="7"/>
       <c r="O37" s="18"/>
       <c r="P37" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q37" s="25">
-        <v>6</v>
-      </c>
-      <c r="R37" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="S37" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="T37" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="U37" s="25" t="s">
-        <v>165</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="Q37" s="25"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="25"/>
+      <c r="T37" s="27"/>
+      <c r="U37" s="25"/>
     </row>
     <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="17"/>
+      <c r="A38" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>178</v>
+      </c>
       <c r="E38" s="16"/>
       <c r="F38" s="18"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="5"/>
+      <c r="G38" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="H38" s="23">
+        <v>30</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
+      <c r="N38" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="25"/>
-      <c r="R38" s="26"/>
-      <c r="S38" s="25"/>
-      <c r="T38" s="27"/>
-      <c r="U38" s="25"/>
+      <c r="P38" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q38" s="25">
+        <v>6</v>
+      </c>
+      <c r="R38" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="S38" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="T38" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="U38" s="25" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="17"/>
+      <c r="A39" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>178</v>
+      </c>
       <c r="E39" s="16"/>
       <c r="F39" s="18"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="5"/>
+      <c r="G39" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="H39" s="23">
+        <v>31</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J39" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
+      <c r="N39" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="25"/>
-      <c r="R39" s="26"/>
-      <c r="S39" s="25"/>
-      <c r="T39" s="27"/>
-      <c r="U39" s="25"/>
+      <c r="P39" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q39" s="25">
+        <v>6</v>
+      </c>
+      <c r="R39" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="S39" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="T39" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="U39" s="25" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
@@ -4466,206 +4596,251 @@
       <c r="T80" s="27"/>
       <c r="U80" s="25"/>
     </row>
-    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="21" t="s">
-        <v>93</v>
-      </c>
-    </row>
+    <row r="81" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="30"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="20"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="5"/>
+      <c r="M81" s="7"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="18"/>
+      <c r="P81" s="18"/>
+      <c r="Q81" s="25"/>
+      <c r="R81" s="26"/>
+      <c r="S81" s="25"/>
+      <c r="T81" s="27"/>
+      <c r="U81" s="25"/>
+    </row>
+    <row r="82" spans="1:21" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="30"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="20"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="7"/>
+      <c r="N82" s="7"/>
+      <c r="O82" s="18"/>
+      <c r="P82" s="18"/>
+      <c r="Q82" s="25"/>
+      <c r="R82" s="26"/>
+      <c r="S82" s="25"/>
+      <c r="T82" s="27"/>
+      <c r="U82" s="25"/>
+    </row>
+    <row r="83" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="21" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="21" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
     </row>
     <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="21" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
     </row>
     <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="21" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4829,12 +5004,6 @@
     <row r="294" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4849,6 +5018,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4859,37 +5034,37 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N36 N38:N80 N3:N34</xm:sqref>
+          <xm:sqref>N38 N40:N82 N3:N36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>P38:P80 K38:K80 P3:P34 K3:K34 I3:I80</xm:sqref>
+          <xm:sqref>P40:P82 K40:K82 P3:P36 K3:K36 I3:I82</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L38:L80 L3:L34</xm:sqref>
+          <xm:sqref>L40:L82 L3:L36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M38:M80 M3:M34</xm:sqref>
+          <xm:sqref>M40:M82 M3:M36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[1]DATOS!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>P35:P37 K35:M37 N35 N37</xm:sqref>
+          <xm:sqref>P37:P39 K37:M39 N37 N39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A80</xm:sqref>
+          <xm:sqref>A3:A82</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>